<commit_message>
I76 mode shapes in thesis
</commit_message>
<xml_diff>
--- a/thesis_doc/draft1/data/modes.xlsx
+++ b/thesis_doc/draft1/data/modes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273BD993-92A1-485E-B858-049EC023977C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,13 +15,20 @@
   <definedNames>
     <definedName name="Superstructure_2Span_1" localSheetId="1">Sheet2!$A$5:$D$246</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Superstructure_2Span" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Superstructure_2Span" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="437" sourceFile="F:\I76\I76\FE Models\Base\Superstructure_2Span.NFL" delimited="0">
       <textFields count="4">
         <textField/>
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="478">
   <si>
     <t>Mode 1</t>
   </si>
@@ -1473,9 +1481,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1586,7 +1594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1594,26 +1602,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1624,12 +1630,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Superstructure_2Span_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Superstructure_2Span_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1675,7 +1684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1708,9 +1717,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1743,6 +1769,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1918,11 +1961,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1956,7 +1999,7 @@
       <c r="N6">
         <v>5</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="14">
         <f>(N6-M6)/M6</f>
         <v>-0.99999874458175531</v>
       </c>
@@ -1965,14 +2008,16 @@
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="16">
         <v>2.7348642500000002</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="12"/>
+      <c r="D7" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="5">
         <f>(C7-B7)/B7</f>
         <v>0.36743212500000011</v>
@@ -1986,7 +2031,7 @@
       <c r="N7">
         <v>0.10404659407899999</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="14">
         <f t="shared" ref="O7:O11" si="0">(N7-M7)/M7</f>
         <v>0.19999999999769319</v>
       </c>
@@ -1995,14 +2040,16 @@
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="15">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="16">
         <v>2.3676324599999998</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="5">
         <f t="shared" ref="F8:F24" si="1">(C8-B8)/B8</f>
         <v>0.16632140886699509</v>
@@ -2016,7 +2063,7 @@
       <c r="N8">
         <v>3982736.44741</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="14">
         <f t="shared" si="0"/>
         <v>-2.2597115874009168E-12</v>
       </c>
@@ -2025,16 +2072,16 @@
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="15">
         <v>2.1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="16">
         <v>3.22170771</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="15">
         <v>2.04327345</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <f>(D9-B9)/B9</f>
         <v>-2.7012642857142877E-2</v>
       </c>
@@ -2051,7 +2098,7 @@
       <c r="N9">
         <v>0.10404659407899999</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="14">
         <f t="shared" si="0"/>
         <v>0.19999999999769319</v>
       </c>
@@ -2060,17 +2107,17 @@
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="15">
         <v>2.44</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="15">
         <v>2.3079333499999999</v>
       </c>
-      <c r="E10" s="14">
-        <f t="shared" ref="E10:E24" si="2">(D10-B10)/B10</f>
+      <c r="E10" s="11">
+        <f t="shared" ref="E10:E23" si="2">(D10-B10)/B10</f>
         <v>-5.4125676229508222E-2</v>
       </c>
       <c r="F10" s="5" t="e">
@@ -2086,7 +2133,7 @@
       <c r="N10">
         <v>100000000</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="14">
         <f t="shared" si="0"/>
         <v>-0.9</v>
       </c>
@@ -2095,14 +2142,16 @@
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="15">
         <v>2.5099999999999998</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -2116,7 +2165,7 @@
       <c r="N11">
         <v>4490368.5510600004</v>
       </c>
-      <c r="O11" s="20">
+      <c r="O11" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2125,16 +2174,16 @@
       <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="15">
         <v>2.54</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="16">
         <v>3.7668420899999999</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="15">
         <v>2.5804058699999999</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="11">
         <f t="shared" si="2"/>
         <v>1.5907822834645608E-2</v>
       </c>
@@ -2147,16 +2196,16 @@
       <c r="A13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="15">
         <v>2.83</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="16">
         <v>3.70763591</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="15">
         <v>2.9505891399999999</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <f t="shared" si="2"/>
         <v>4.2611003533568857E-2</v>
       </c>
@@ -2169,14 +2218,16 @@
       <c r="A14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="15">
         <v>2.93</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="14"/>
+      <c r="D14" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="11"/>
       <c r="F14" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -2186,16 +2237,16 @@
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="15">
         <v>3.2</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="15">
         <v>3.4451671799999999</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <f t="shared" si="2"/>
         <v>7.6614743749999908E-2</v>
       </c>
@@ -2208,14 +2259,16 @@
       <c r="A16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="15">
         <v>3.34</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="16">
         <v>4.5809138200000001</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="11"/>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>0.37153108383233541</v>
@@ -2225,16 +2278,16 @@
       <c r="A17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="15">
         <v>3.52</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="15">
         <v>3.6538124600000002</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <f t="shared" si="2"/>
         <v>3.8014903409090944E-2</v>
       </c>
@@ -2247,16 +2300,16 @@
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="15">
         <v>3.56</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="16">
         <v>4.2451704399999999</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="15">
         <v>4.05668235</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="11">
         <f t="shared" si="2"/>
         <v>0.13951751404494381</v>
       </c>
@@ -2266,19 +2319,19 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="17">
         <v>3.56</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>4.0651109400000003</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="13">
         <f t="shared" si="2"/>
         <v>0.14188509550561804</v>
       </c>
@@ -2398,11 +2451,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D482"/>
   <sheetViews>
     <sheetView topLeftCell="A168" workbookViewId="0">
@@ -4976,7 +5030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>